<commit_message>
fix a few charts
</commit_message>
<xml_diff>
--- a/todo_list.xlsx
+++ b/todo_list.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$56</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="75">
   <si>
     <t>To Do List</t>
   </si>
@@ -234,6 +234,27 @@
   </si>
   <si>
     <t>update report links</t>
+  </si>
+  <si>
+    <t>make dots darker in maps?</t>
+  </si>
+  <si>
+    <t>Ask Mal????</t>
+  </si>
+  <si>
+    <t>note that this is a proportion in ward map</t>
+  </si>
+  <si>
+    <t>fix scale on ward distros</t>
+  </si>
+  <si>
+    <t>change colors of pull quotes</t>
+  </si>
+  <si>
+    <t>chart margins</t>
+  </si>
+  <si>
+    <t>remove ticks from axis</t>
   </si>
 </sst>
 </file>
@@ -588,11 +609,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:C21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -784,15 +803,35 @@
         <v>4</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
@@ -800,90 +839,46 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>39</v>
@@ -894,24 +889,24 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -919,205 +914,244 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>5</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B38" t="s">
         <v>6</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>55</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B39" t="s">
         <v>6</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C39" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>56</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B40" t="s">
         <v>6</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>57</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B41" t="s">
         <v>6</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C41" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>51</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B42" t="s">
         <v>52</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C42" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>17</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B44" t="s">
         <v>16</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>64</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B45" t="s">
         <v>39</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C45" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>63</v>
       </c>
-      <c r="B40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="E47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
         <v>20</v>
@@ -1128,7 +1162,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B53" t="s">
         <v>20</v>
@@ -1139,7 +1173,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B54" t="s">
         <v>20</v>
@@ -1148,40 +1182,106 @@
         <v>9</v>
       </c>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B57" t="s">
-        <v>48</v>
+        <v>20</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>20</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>54</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B66" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C67"/>
+  <autoFilter ref="C1:C73"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add names to ward map
</commit_message>
<xml_diff>
--- a/todo_list.xlsx
+++ b/todo_list.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="83">
   <si>
     <t>To Do List</t>
   </si>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,7 +860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -874,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -888,7 +888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -902,7 +902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -916,7 +916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -930,7 +930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -944,7 +944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -958,7 +958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -972,37 +972,92 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
@@ -1012,53 +1067,6 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>51</v>
@@ -1103,51 +1111,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" t="s">
-        <v>63</v>
-      </c>
-    </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="E47" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1208,17 +1183,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>32</v>
       </c>
-      <c r="B57" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add a bunch of stuff.........mobile dot improvement, map improvements
</commit_message>
<xml_diff>
--- a/todo_list.xlsx
+++ b/todo_list.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="106">
   <si>
     <t>To Do List</t>
   </si>
@@ -284,9 +284,6 @@
     <t xml:space="preserve">make end dots pulse once? </t>
   </si>
   <si>
-    <t>text DEE~~!</t>
-  </si>
-  <si>
     <t>apply Forney copy edits</t>
   </si>
   <si>
@@ -306,6 +303,51 @@
   </si>
   <si>
     <t>update google tags</t>
+  </si>
+  <si>
+    <t>final checklist</t>
+  </si>
+  <si>
+    <t>https://urbanorg.app.box.com/notes/62041029749</t>
+  </si>
+  <si>
+    <t>add in the date</t>
+  </si>
+  <si>
+    <t>make sure date is correct</t>
+  </si>
+  <si>
+    <t>add note to neighborhood chart</t>
+  </si>
+  <si>
+    <t>Notes: Urban Institute analysis of student-level data. A student’s neighborhood is defined as the student’s home census tract.</t>
+  </si>
+  <si>
+    <t>improve ward map overflow tooltip issue</t>
+  </si>
+  <si>
+    <t>favicon</t>
+  </si>
+  <si>
+    <t>should text under maps say "Note"?</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>change distro chart labels to blue</t>
+  </si>
+  <si>
+    <t>change distro chart labels to straight and above the thing</t>
+  </si>
+  <si>
+    <t>make the axis less crowded on mobile</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>reduce height on mobile</t>
   </si>
 </sst>
 </file>
@@ -361,8 +403,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -376,15 +422,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -660,9 +710,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1044,13 +1096,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1063,10 +1118,13 @@
       <c r="C29" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
@@ -1074,48 +1132,102 @@
       <c r="C30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" t="s">
-        <v>9</v>
+      <c r="D30" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="E32" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1173,6 +1285,17 @@
         <v>35</v>
       </c>
     </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>65</v>
@@ -1187,9 +1310,20 @@
         <v>75</v>
       </c>
     </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>12</v>
@@ -1200,7 +1334,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>12</v>
@@ -1211,7 +1345,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
@@ -1245,7 +1379,7 @@
         <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1284,6 +1418,20 @@
         <v>33</v>
       </c>
     </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
@@ -1504,6 +1652,29 @@
       </c>
       <c r="B82" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>102</v>
+      </c>
+      <c r="B85" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust icons and stuff
</commit_message>
<xml_diff>
--- a/todo_list.xlsx
+++ b/todo_list.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$80</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="107">
   <si>
     <t>To Do List</t>
   </si>
@@ -131,9 +131,6 @@
     <t>update social media buttons</t>
   </si>
   <si>
-    <t>talk to team</t>
-  </si>
-  <si>
     <t>Update Mapbox design</t>
   </si>
   <si>
@@ -348,6 +345,12 @@
   </si>
   <si>
     <t>reduce height on mobile</t>
+  </si>
+  <si>
+    <t>half</t>
+  </si>
+  <si>
+    <t>Nicole</t>
   </si>
 </sst>
 </file>
@@ -710,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,7 +740,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -812,13 +815,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -835,7 +838,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -849,7 +852,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -883,10 +886,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -925,7 +928,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -939,10 +942,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -953,10 +956,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>9</v>
@@ -967,10 +970,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
@@ -981,10 +984,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
@@ -995,7 +998,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>12</v>
@@ -1009,10 +1012,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>9</v>
@@ -1023,7 +1026,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>12</v>
@@ -1037,10 +1040,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -1051,10 +1054,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -1065,27 +1068,27 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>9</v>
@@ -1096,7 +1099,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -1110,10 +1113,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>9</v>
@@ -1124,7 +1127,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
@@ -1133,43 +1136,80 @@
         <v>9</v>
       </c>
       <c r="D30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" t="s">
-        <v>96</v>
+        <v>88</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1182,140 +1222,133 @@
       <c r="C36" t="s">
         <v>9</v>
       </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" t="s">
-        <v>18</v>
+        <v>34</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E42" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C46" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
@@ -1323,297 +1356,212 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>90</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>28</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" t="s">
-        <v>9</v>
+        <v>90</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="E55" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>35</v>
-      </c>
-      <c r="E57" t="s">
-        <v>100</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>80</v>
-      </c>
-      <c r="B59" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" t="s">
-        <v>48</v>
-      </c>
-      <c r="C60" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" t="s">
         <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
         <v>6</v>
       </c>
-      <c r="C63" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>78</v>
+      </c>
+      <c r="B68" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>67</v>
       </c>
-      <c r="B64" t="s">
-        <v>37</v>
-      </c>
-      <c r="C64" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" t="s">
-        <v>37</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B73" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>19</v>
-      </c>
-      <c r="B68" t="s">
-        <v>20</v>
-      </c>
-      <c r="C68" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>21</v>
-      </c>
-      <c r="B69" t="s">
-        <v>20</v>
-      </c>
-      <c r="C69" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>22</v>
-      </c>
-      <c r="B70" t="s">
-        <v>20</v>
-      </c>
-      <c r="C70" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" t="s">
-        <v>20</v>
-      </c>
-      <c r="C71" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>24</v>
-      </c>
-      <c r="B72" t="s">
-        <v>20</v>
-      </c>
-      <c r="C72" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>39</v>
-      </c>
-      <c r="B73" t="s">
-        <v>20</v>
-      </c>
-      <c r="C73" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>41</v>
-      </c>
-      <c r="B74" t="s">
-        <v>20</v>
-      </c>
-      <c r="C74" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>42</v>
-      </c>
-      <c r="B75" t="s">
-        <v>20</v>
-      </c>
-      <c r="C75" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>43</v>
       </c>
       <c r="B76" t="s">
         <v>20</v>
@@ -1622,63 +1570,151 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>21</v>
+      </c>
+      <c r="B77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>38</v>
+      </c>
+      <c r="B81" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>40</v>
+      </c>
+      <c r="B82" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>41</v>
+      </c>
+      <c r="B83" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>48</v>
+      </c>
+      <c r="B87" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>43</v>
+      </c>
+      <c r="B88" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>46</v>
+      </c>
+      <c r="B89" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>49</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B90" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>44</v>
-      </c>
-      <c r="B80" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>47</v>
-      </c>
-      <c r="B81" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>50</v>
-      </c>
-      <c r="B82" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="B93" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>102</v>
       </c>
-      <c r="B85" t="s">
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>105</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="C1:C89"/>
+  <autoFilter ref="C1:C97"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change name and some style edits
</commit_message>
<xml_diff>
--- a/todo_list.xlsx
+++ b/todo_list.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="110">
   <si>
     <t>To Do List</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>update data link</t>
+  </si>
+  <si>
+    <t>check webkit animation for pulse…work in firefox, etc?</t>
   </si>
 </sst>
 </file>
@@ -729,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1514,6 +1517,17 @@
         <v>34</v>
       </c>
     </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
remove a pic and add a gif
</commit_message>
<xml_diff>
--- a/todo_list.xlsx
+++ b/todo_list.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="117">
   <si>
     <t>To Do List</t>
   </si>
@@ -372,13 +372,22 @@
   </si>
   <si>
     <t>set staging redirect</t>
+  </si>
+  <si>
+    <t>update github name</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>make india dot at top not have jenky opacity issues</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -405,6 +414,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -446,9 +462,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -744,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:C65"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1418,12 +1436,74 @@
         <v>4</v>
       </c>
     </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>98</v>
+      </c>
+    </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C52" t="s">
         <v>9</v>
@@ -1434,10 +1514,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
@@ -1448,58 +1528,52 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" t="s">
         <v>9</v>
       </c>
       <c r="D54" t="s">
         <v>4</v>
       </c>
       <c r="E54" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>34</v>
-      </c>
-      <c r="E55" t="s">
-        <v>98</v>
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>95</v>
-      </c>
-      <c r="B57" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="D57" t="s">
         <v>4</v>
@@ -1507,7 +1581,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="B58" t="s">
         <v>16</v>
@@ -1515,35 +1589,29 @@
       <c r="C58" t="s">
         <v>9</v>
       </c>
-      <c r="E58" t="s">
-        <v>90</v>
+      <c r="D58" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>105</v>
-      </c>
-      <c r="B59" t="s">
-        <v>12</v>
-      </c>
-      <c r="C59" t="s">
-        <v>9</v>
+        <v>114</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>106</v>
-      </c>
-      <c r="B60" t="s">
-        <v>12</v>
-      </c>
-      <c r="C60" t="s">
-        <v>34</v>
+        <v>58</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
@@ -1551,94 +1619,143 @@
       <c r="C61" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>112</v>
-      </c>
-      <c r="B62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" t="s">
-        <v>34</v>
+      <c r="D61" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>110</v>
-      </c>
-      <c r="B63" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>111</v>
-      </c>
-      <c r="D64" t="s">
-        <v>4</v>
+        <v>106</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="A71" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E71" t="s">
+      <c r="D71" s="2"/>
+      <c r="E71" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="A72" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D72" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E72" s="2"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="A73" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="A74" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">

</xml_diff>